<commit_message>
add comments and leaders att
</commit_message>
<xml_diff>
--- a/Data/Results/itog.xlsx
+++ b/Data/Results/itog.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M53"/>
+  <dimension ref="A1:N53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,163 +434,177 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>ФИО</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Собрания (присутствие на ежемесячных собраниях ПБ3)</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Меро ПБ (организация или активное принятие в организации мероприятия внутри пб3)</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Меро ППОСА (организация или активное принятие в организации мероприятия внутри ППОСА ГУАП или на межвузовском уровне)</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Поручения (выполнение поручений от пб3 и посещение различных форумов от лица пб3)</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Волонтёрство</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Должность (занимаемая должность в структуре пб3)</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Дизайн (создание картинки к посту в соц.сетях пб3)</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Текст (написание текста к посту в соц.сетях пб3)</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Видео</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Руководство в проекте (занимаение должности руководителя в проекте профкома)</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Ответственный за офис</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Всего</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>Муравьева Алина Алексеевна</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
-      <c r="G2" t="n">
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="n">
         <v>16</v>
       </c>
-      <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>Кириллова Наталья Романовна</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
-      <c r="G3" t="n">
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="n">
         <v>16</v>
       </c>
-      <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>Ворожцов Андрей Ильич</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
-      <c r="G4" t="n">
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="n">
         <v>16</v>
       </c>
-      <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>Фишков Максим Романович</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
-      <c r="G5" t="n">
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="n">
         <v>16</v>
       </c>
-      <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>Лобанов Егор Олегович</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
@@ -602,14 +616,17 @@
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
       <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
         <is>
           <t>Ерина Лилия Александровна</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
@@ -621,14 +638,17 @@
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
         <is>
           <t>Мурзашева Татьяна Александровна</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
@@ -640,14 +660,17 @@
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
       <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
         <is>
           <t>Кунакаева Милена Тимуровна</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
@@ -659,35 +682,43 @@
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
         <is>
           <t>Томский Алексей Андреевич</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
-      <c r="G10" t="n">
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="n">
         <v>16</v>
       </c>
-      <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
+      <c r="L10" t="n">
+        <v>16</v>
+      </c>
       <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
         <is>
           <t>Агеев Даниил Олегович</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
@@ -699,14 +730,17 @@
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
         <is>
           <t>Батайкин Георгий Александрович</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
@@ -718,14 +752,17 @@
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
         <is>
           <t>Борисенко Даниил Евгеньевич</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
@@ -737,14 +774,17 @@
       <c r="K13" t="inlineStr"/>
       <c r="L13" t="inlineStr"/>
       <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
         <is>
           <t>Гвоздев Илья Игоревич</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
@@ -756,14 +796,17 @@
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr"/>
       <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
         <is>
           <t>Горган Марьяна Сергеевна</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
@@ -775,14 +818,17 @@
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="inlineStr"/>
+      <c r="N15" t="inlineStr"/>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
         <is>
           <t>Горяинов Валерий Алексеевич</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
@@ -794,35 +840,41 @@
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr"/>
       <c r="M16" t="inlineStr"/>
+      <c r="N16" t="inlineStr"/>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
         <is>
           <t>Дементьева Виктория Евгеньевна</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
-      <c r="G17" t="n">
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="n">
         <v>16</v>
       </c>
-      <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr"/>
       <c r="K17" t="inlineStr"/>
       <c r="L17" t="inlineStr"/>
       <c r="M17" t="inlineStr"/>
+      <c r="N17" t="inlineStr"/>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
         <is>
           <t>Дмитриев Егор Филиппович</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr"/>
@@ -834,14 +886,17 @@
       <c r="K18" t="inlineStr"/>
       <c r="L18" t="inlineStr"/>
       <c r="M18" t="inlineStr"/>
+      <c r="N18" t="inlineStr"/>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
         <is>
           <t>Евтушенко Валерия Германовна</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr"/>
@@ -853,14 +908,17 @@
       <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr"/>
       <c r="M19" t="inlineStr"/>
+      <c r="N19" t="inlineStr"/>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
         <is>
           <t>Казбанов Кирилл Николаевич</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
@@ -872,14 +930,17 @@
       <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="inlineStr"/>
+      <c r="N20" t="inlineStr"/>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
         <is>
           <t>Каримова Зарнигор Шухратовна</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
@@ -891,14 +952,17 @@
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr"/>
       <c r="M21" t="inlineStr"/>
+      <c r="N21" t="inlineStr"/>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
         <is>
           <t>Коваленко Михаил Андреевич</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr"/>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr"/>
@@ -910,14 +974,17 @@
       <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr"/>
       <c r="M22" t="inlineStr"/>
+      <c r="N22" t="inlineStr"/>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
         <is>
           <t>Комаров Максим Сергеевич</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr"/>
@@ -929,14 +996,17 @@
       <c r="K23" t="inlineStr"/>
       <c r="L23" t="inlineStr"/>
       <c r="M23" t="inlineStr"/>
+      <c r="N23" t="inlineStr"/>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
         <is>
           <t>Коробкин Кирилл Максимович</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr"/>
@@ -948,35 +1018,41 @@
       <c r="K24" t="inlineStr"/>
       <c r="L24" t="inlineStr"/>
       <c r="M24" t="inlineStr"/>
+      <c r="N24" t="inlineStr"/>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
         <is>
           <t>Королев Иван Михайлович</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr"/>
-      <c r="G25" t="n">
+      <c r="G25" t="inlineStr"/>
+      <c r="H25" t="n">
         <v>16</v>
       </c>
-      <c r="H25" t="inlineStr"/>
       <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr"/>
       <c r="M25" t="inlineStr"/>
+      <c r="N25" t="inlineStr"/>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
         <is>
           <t>Кочнев Олег Евгеньевич</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr"/>
       <c r="C26" t="inlineStr"/>
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr"/>
@@ -988,14 +1064,17 @@
       <c r="K26" t="inlineStr"/>
       <c r="L26" t="inlineStr"/>
       <c r="M26" t="inlineStr"/>
+      <c r="N26" t="inlineStr"/>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
         <is>
           <t>Кривулин Кирилл Сергеевич</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr"/>
       <c r="C27" t="inlineStr"/>
       <c r="D27" t="inlineStr"/>
       <c r="E27" t="inlineStr"/>
@@ -1007,14 +1086,17 @@
       <c r="K27" t="inlineStr"/>
       <c r="L27" t="inlineStr"/>
       <c r="M27" t="inlineStr"/>
+      <c r="N27" t="inlineStr"/>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
         <is>
           <t>Кузьменок Артем Андреевич</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr"/>
@@ -1026,14 +1108,17 @@
       <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr"/>
       <c r="M28" t="inlineStr"/>
+      <c r="N28" t="inlineStr"/>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
         <is>
           <t>Куличёв Артём Дмитриевич</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr"/>
       <c r="C29" t="inlineStr"/>
       <c r="D29" t="inlineStr"/>
       <c r="E29" t="inlineStr"/>
@@ -1045,14 +1130,17 @@
       <c r="K29" t="inlineStr"/>
       <c r="L29" t="inlineStr"/>
       <c r="M29" t="inlineStr"/>
+      <c r="N29" t="inlineStr"/>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
         <is>
           <t>Курашов Дмитрий Евгеньевич</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr"/>
       <c r="C30" t="inlineStr"/>
       <c r="D30" t="inlineStr"/>
       <c r="E30" t="inlineStr"/>
@@ -1064,14 +1152,17 @@
       <c r="K30" t="inlineStr"/>
       <c r="L30" t="inlineStr"/>
       <c r="M30" t="inlineStr"/>
+      <c r="N30" t="inlineStr"/>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
         <is>
           <t>Мазов Роман Юрьевич</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr"/>
       <c r="C31" t="inlineStr"/>
       <c r="D31" t="inlineStr"/>
       <c r="E31" t="inlineStr"/>
@@ -1083,14 +1174,17 @@
       <c r="K31" t="inlineStr"/>
       <c r="L31" t="inlineStr"/>
       <c r="M31" t="inlineStr"/>
+      <c r="N31" t="inlineStr"/>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
         <is>
           <t>Моцная Татьяна Вячеславовна</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr"/>
       <c r="C32" t="inlineStr"/>
       <c r="D32" t="inlineStr"/>
       <c r="E32" t="inlineStr"/>
@@ -1102,14 +1196,17 @@
       <c r="K32" t="inlineStr"/>
       <c r="L32" t="inlineStr"/>
       <c r="M32" t="inlineStr"/>
+      <c r="N32" t="inlineStr"/>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
         <is>
           <t>Мясников Павел Сергеевич</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr"/>
       <c r="C33" t="inlineStr"/>
       <c r="D33" t="inlineStr"/>
       <c r="E33" t="inlineStr"/>
@@ -1121,14 +1218,17 @@
       <c r="K33" t="inlineStr"/>
       <c r="L33" t="inlineStr"/>
       <c r="M33" t="inlineStr"/>
+      <c r="N33" t="inlineStr"/>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
         <is>
           <t>Нафиков Дамир Евгеньевич</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr"/>
       <c r="C34" t="inlineStr"/>
       <c r="D34" t="inlineStr"/>
       <c r="E34" t="inlineStr"/>
@@ -1140,14 +1240,17 @@
       <c r="K34" t="inlineStr"/>
       <c r="L34" t="inlineStr"/>
       <c r="M34" t="inlineStr"/>
+      <c r="N34" t="inlineStr"/>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
         <is>
           <t>Немцев Константин Николаевич</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr"/>
       <c r="C35" t="inlineStr"/>
       <c r="D35" t="inlineStr"/>
       <c r="E35" t="inlineStr"/>
@@ -1159,14 +1262,17 @@
       <c r="K35" t="inlineStr"/>
       <c r="L35" t="inlineStr"/>
       <c r="M35" t="inlineStr"/>
+      <c r="N35" t="inlineStr"/>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
         <is>
           <t>Охонская Анна Игоревна</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr"/>
       <c r="C36" t="inlineStr"/>
       <c r="D36" t="inlineStr"/>
       <c r="E36" t="inlineStr"/>
@@ -1178,14 +1284,17 @@
       <c r="K36" t="inlineStr"/>
       <c r="L36" t="inlineStr"/>
       <c r="M36" t="inlineStr"/>
+      <c r="N36" t="inlineStr"/>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
         <is>
           <t>Павлова Елизавета Сергеевна</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr"/>
       <c r="C37" t="inlineStr"/>
       <c r="D37" t="inlineStr"/>
       <c r="E37" t="inlineStr"/>
@@ -1197,14 +1306,17 @@
       <c r="K37" t="inlineStr"/>
       <c r="L37" t="inlineStr"/>
       <c r="M37" t="inlineStr"/>
+      <c r="N37" t="inlineStr"/>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
         <is>
           <t>Подласова Алиса Романовна</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr"/>
       <c r="C38" t="inlineStr"/>
       <c r="D38" t="inlineStr"/>
       <c r="E38" t="inlineStr"/>
@@ -1216,14 +1328,17 @@
       <c r="K38" t="inlineStr"/>
       <c r="L38" t="inlineStr"/>
       <c r="M38" t="inlineStr"/>
+      <c r="N38" t="inlineStr"/>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr">
         <is>
           <t>Попова Алёна Романовна</t>
         </is>
       </c>
-      <c r="B39" t="inlineStr"/>
       <c r="C39" t="inlineStr"/>
       <c r="D39" t="inlineStr"/>
       <c r="E39" t="inlineStr"/>
@@ -1233,16 +1348,21 @@
       <c r="I39" t="inlineStr"/>
       <c r="J39" t="inlineStr"/>
       <c r="K39" t="inlineStr"/>
-      <c r="L39" t="inlineStr"/>
+      <c r="L39" t="n">
+        <v>16</v>
+      </c>
       <c r="M39" t="inlineStr"/>
+      <c r="N39" t="inlineStr"/>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr">
         <is>
           <t>Порошина Мария Андреевна</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr"/>
       <c r="C40" t="inlineStr"/>
       <c r="D40" t="inlineStr"/>
       <c r="E40" t="inlineStr"/>
@@ -1254,14 +1374,17 @@
       <c r="K40" t="inlineStr"/>
       <c r="L40" t="inlineStr"/>
       <c r="M40" t="inlineStr"/>
+      <c r="N40" t="inlineStr"/>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="inlineStr">
         <is>
           <t>Пфайфер Алина Михайловна</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr"/>
       <c r="C41" t="inlineStr"/>
       <c r="D41" t="inlineStr"/>
       <c r="E41" t="inlineStr"/>
@@ -1273,14 +1396,17 @@
       <c r="K41" t="inlineStr"/>
       <c r="L41" t="inlineStr"/>
       <c r="M41" t="inlineStr"/>
+      <c r="N41" t="inlineStr"/>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="inlineStr">
         <is>
           <t>Рябухин Владислав Александрович</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr"/>
       <c r="C42" t="inlineStr"/>
       <c r="D42" t="inlineStr"/>
       <c r="E42" t="inlineStr"/>
@@ -1292,14 +1418,17 @@
       <c r="K42" t="inlineStr"/>
       <c r="L42" t="inlineStr"/>
       <c r="M42" t="inlineStr"/>
+      <c r="N42" t="inlineStr"/>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="inlineStr">
         <is>
           <t>Соболев Михаил Романович</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr"/>
       <c r="C43" t="inlineStr"/>
       <c r="D43" t="inlineStr"/>
       <c r="E43" t="inlineStr"/>
@@ -1311,35 +1440,43 @@
       <c r="K43" t="inlineStr"/>
       <c r="L43" t="inlineStr"/>
       <c r="M43" t="inlineStr"/>
+      <c r="N43" t="inlineStr"/>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="inlineStr">
         <is>
           <t>Стогова Александра Алексеевна</t>
         </is>
       </c>
-      <c r="B44" t="inlineStr"/>
       <c r="C44" t="inlineStr"/>
       <c r="D44" t="inlineStr"/>
       <c r="E44" t="inlineStr"/>
       <c r="F44" t="inlineStr"/>
-      <c r="G44" t="n">
+      <c r="G44" t="inlineStr"/>
+      <c r="H44" t="n">
         <v>16</v>
       </c>
-      <c r="H44" t="inlineStr"/>
       <c r="I44" t="inlineStr"/>
       <c r="J44" t="inlineStr"/>
       <c r="K44" t="inlineStr"/>
-      <c r="L44" t="inlineStr"/>
+      <c r="L44" t="n">
+        <v>16</v>
+      </c>
       <c r="M44" t="inlineStr"/>
+      <c r="N44" t="inlineStr"/>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="inlineStr">
         <is>
           <t>Тарасова Виктория Константиновна</t>
         </is>
       </c>
-      <c r="B45" t="inlineStr"/>
       <c r="C45" t="inlineStr"/>
       <c r="D45" t="inlineStr"/>
       <c r="E45" t="inlineStr"/>
@@ -1351,14 +1488,17 @@
       <c r="K45" t="inlineStr"/>
       <c r="L45" t="inlineStr"/>
       <c r="M45" t="inlineStr"/>
+      <c r="N45" t="inlineStr"/>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="inlineStr">
         <is>
           <t>Терешкин Ярослав Станиславович</t>
         </is>
       </c>
-      <c r="B46" t="inlineStr"/>
       <c r="C46" t="inlineStr"/>
       <c r="D46" t="inlineStr"/>
       <c r="E46" t="inlineStr"/>
@@ -1370,14 +1510,17 @@
       <c r="K46" t="inlineStr"/>
       <c r="L46" t="inlineStr"/>
       <c r="M46" t="inlineStr"/>
+      <c r="N46" t="inlineStr"/>
     </row>
     <row r="47">
-      <c r="A47" t="inlineStr">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="inlineStr">
         <is>
           <t>Тетин Никита Олегович</t>
         </is>
       </c>
-      <c r="B47" t="inlineStr"/>
       <c r="C47" t="inlineStr"/>
       <c r="D47" t="inlineStr"/>
       <c r="E47" t="inlineStr"/>
@@ -1389,14 +1532,17 @@
       <c r="K47" t="inlineStr"/>
       <c r="L47" t="inlineStr"/>
       <c r="M47" t="inlineStr"/>
+      <c r="N47" t="inlineStr"/>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="inlineStr">
         <is>
           <t>Ульрих Антон Александрович</t>
         </is>
       </c>
-      <c r="B48" t="inlineStr"/>
       <c r="C48" t="inlineStr"/>
       <c r="D48" t="inlineStr"/>
       <c r="E48" t="inlineStr"/>
@@ -1408,35 +1554,43 @@
       <c r="K48" t="inlineStr"/>
       <c r="L48" t="inlineStr"/>
       <c r="M48" t="inlineStr"/>
+      <c r="N48" t="inlineStr"/>
     </row>
     <row r="49">
-      <c r="A49" t="inlineStr">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="inlineStr">
         <is>
           <t>Хвастунов Александр Алексеевич</t>
         </is>
       </c>
-      <c r="B49" t="inlineStr"/>
       <c r="C49" t="inlineStr"/>
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="inlineStr"/>
       <c r="F49" t="inlineStr"/>
-      <c r="G49" t="n">
+      <c r="G49" t="inlineStr"/>
+      <c r="H49" t="n">
         <v>16</v>
       </c>
-      <c r="H49" t="inlineStr"/>
       <c r="I49" t="inlineStr"/>
       <c r="J49" t="inlineStr"/>
       <c r="K49" t="inlineStr"/>
-      <c r="L49" t="inlineStr"/>
+      <c r="L49" t="n">
+        <v>16</v>
+      </c>
       <c r="M49" t="inlineStr"/>
+      <c r="N49" t="inlineStr"/>
     </row>
     <row r="50">
-      <c r="A50" t="inlineStr">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="inlineStr">
         <is>
           <t>Шакиров Амир Мисхатович</t>
         </is>
       </c>
-      <c r="B50" t="inlineStr"/>
       <c r="C50" t="inlineStr"/>
       <c r="D50" t="inlineStr"/>
       <c r="E50" t="inlineStr"/>
@@ -1448,14 +1602,17 @@
       <c r="K50" t="inlineStr"/>
       <c r="L50" t="inlineStr"/>
       <c r="M50" t="inlineStr"/>
+      <c r="N50" t="inlineStr"/>
     </row>
     <row r="51">
-      <c r="A51" t="inlineStr">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="inlineStr">
         <is>
           <t>Шамсутдинов Марк Эдуардович</t>
         </is>
       </c>
-      <c r="B51" t="inlineStr"/>
       <c r="C51" t="inlineStr"/>
       <c r="D51" t="inlineStr"/>
       <c r="E51" t="inlineStr"/>
@@ -1467,14 +1624,17 @@
       <c r="K51" t="inlineStr"/>
       <c r="L51" t="inlineStr"/>
       <c r="M51" t="inlineStr"/>
+      <c r="N51" t="inlineStr"/>
     </row>
     <row r="52">
-      <c r="A52" t="inlineStr">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="inlineStr">
         <is>
           <t>Шыхалиев Эльмир Ильхам оглы</t>
         </is>
       </c>
-      <c r="B52" t="inlineStr"/>
       <c r="C52" t="inlineStr"/>
       <c r="D52" t="inlineStr"/>
       <c r="E52" t="inlineStr"/>
@@ -1486,14 +1646,17 @@
       <c r="K52" t="inlineStr"/>
       <c r="L52" t="inlineStr"/>
       <c r="M52" t="inlineStr"/>
+      <c r="N52" t="inlineStr"/>
     </row>
     <row r="53">
-      <c r="A53" t="inlineStr">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="inlineStr">
         <is>
           <t>Шкроб Алексей Иванович</t>
         </is>
       </c>
-      <c r="B53" t="inlineStr"/>
       <c r="C53" t="inlineStr"/>
       <c r="D53" t="inlineStr"/>
       <c r="E53" t="inlineStr"/>
@@ -1505,6 +1668,7 @@
       <c r="K53" t="inlineStr"/>
       <c r="L53" t="inlineStr"/>
       <c r="M53" t="inlineStr"/>
+      <c r="N53" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>